<commit_message>
update api export file
</commit_message>
<xml_diff>
--- a/server-database/export/TemplateInfoPerson.xlsx
+++ b/server-database/export/TemplateInfoPerson.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Last Name</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Nhat</t>
   </si>
   <si>
-    <t xml:space="preserve"> Nguyen Trong</t>
+    <t>Nguyen Trong</t>
   </si>
   <si>
     <t>Nguyen Trong Nhat</t>
@@ -49,9 +49,6 @@
     <t>Nhat1</t>
   </si>
   <si>
-    <t xml:space="preserve"> Nguyen Trong1</t>
-  </si>
-  <si>
     <t>Nguyen Trong Nhat1</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>Nhat2</t>
   </si>
   <si>
-    <t xml:space="preserve"> Nguyen Trong2</t>
-  </si>
-  <si>
     <t>Nguyen Trong Nhat2</t>
   </si>
   <si>
@@ -76,12 +70,6 @@
     <t>Ha Noi2</t>
   </si>
   <si>
-    <t>Nhat3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nguyen Trong3</t>
-  </si>
-  <si>
     <t>Nguyen Trong Nhat3</t>
   </si>
   <si>
@@ -89,21 +77,6 @@
   </si>
   <si>
     <t>Ha Noi3</t>
-  </si>
-  <si>
-    <t>Nhat4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nguyen Trong4</t>
-  </si>
-  <si>
-    <t>Nguyen Trong Nhat4</t>
-  </si>
-  <si>
-    <t>01234564</t>
-  </si>
-  <si>
-    <t>Ha Noi4</t>
   </si>
 </sst>
 </file>
@@ -455,67 +428,50 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>